<commit_message>
PRODUCT ADD, UPDATE API DOCUMENTATION
</commit_message>
<xml_diff>
--- a/API Docs.xlsx
+++ b/API Docs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>API ENDPOINT</t>
   </si>
@@ -330,6 +330,116 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>product/{id}</t>
+  </si>
+  <si>
+    <t>/product</t>
+  </si>
+  <si>
+    <t>{
+    "name": "DROID BLACK",
+    "distImportDate": "2021-05-09",
+    "shopImportDate": "2021-05-09",
+    "categoryId": "2",
+    "variants": [
+        {
+        "code": "vip-droid-black",
+        "mrp": "4020",
+        "discount": "50",
+        "size": "large",
+        "colour": "black"
+    }]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "data": [
+        {
+            "createdAt": "2021-05-09T19:10:36.976+00:00",
+            "createdBy": null,
+            "updatedAt": "2021-05-09T19:10:36.976+00:00",
+            "updatedBy": null,
+            "id": 5,
+            "name": "DROID GREY",
+            "distImportDate": "2021-05-09",
+            "shopImportDate": "2021-05-09",
+            "variants": [
+                {
+                    "createdAt": "2021-05-09T19:10:37.042+00:00",
+                    "createdBy": null,
+                    "updatedAt": "2021-05-09T19:10:37.042+00:00",
+                    "updatedBy": null,
+                    "id": 5,
+                    "code": "vip-droid-grey",
+                    "mrp": 4020,
+                    "discount": 20,
+                    "size": "large",
+                    "colour": "grey"
+                }
+            ]
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "name": "DROID BLACK",
+    "distImportDate": "2021-05-09",
+    "shopImportDate": "2021-05-09",
+    "categoryId": "2",
+    "variants": [
+        {
+        "id": 2,
+        "code": "vip-droid-black",
+        "mrp": "4020",
+        "discount": "30",
+        "size": "large",
+        "colour": "black"
+    }]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "data": [
+        {
+            "createdAt": "2021-05-09T09:13:13.000+00:00",
+            "createdBy": null,
+            "updatedAt": "2021-05-09T19:13:53.342+00:00",
+            "updatedBy": null,
+            "id": 3,
+            "name": "DROID BLACK",
+            "distImportDate": "2021-05-09",
+            "shopImportDate": "2021-05-09",
+            "variants": [
+                {
+                    "createdAt": null,
+                    "createdBy": null,
+                    "updatedAt": "2021-05-09T19:13:53.343+00:00",
+                    "updatedBy": null,
+                    "id": 2,
+                    "code": "vip-droid-black",
+                    "mrp": 4020,
+                    "discount": 30,
+                    "size": "large",
+                    "colour": "black"
+                }
+            ]
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>200
+404
+400</t>
+  </si>
+  <si>
+    <t>200
+404</t>
   </si>
 </sst>
 </file>
@@ -421,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -458,6 +568,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -741,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,6 +1048,62 @@
       <c r="E12" s="12"/>
       <c r="F12" s="11"/>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="17" spans="1:6" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>22</v>

</xml_diff>